<commit_message>
update vmax for store model
</commit_message>
<xml_diff>
--- a/Model_Parameters Store model.xlsx
+++ b/Model_Parameters Store model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oweisberg\Documents\GitHub\recycle_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA72F11C-81B4-4B09-A104-D90780AE1E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CACF7C-17F2-400A-AD72-DB1D71AF9291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="135">
   <si>
     <t>Mh</t>
   </si>
@@ -424,13 +424,31 @@
   </si>
   <si>
     <t>OverflowMode</t>
+  </si>
+  <si>
+    <t>ROSMode</t>
+  </si>
+  <si>
+    <t>is ROS enabled</t>
+  </si>
+  <si>
+    <t>omegaP</t>
+  </si>
+  <si>
+    <t>1 / µmol/L</t>
+  </si>
+  <si>
+    <t>growth penalty of ROS</t>
+  </si>
+  <si>
+    <t>omegaH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,6 +476,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -473,7 +496,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -610,11 +633,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -686,6 +720,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -990,13 +1030,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S59"/>
+  <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" style="1" customWidth="1"/>
@@ -1011,7 +1052,7 @@
     <col min="15" max="17" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="11" customFormat="1" ht="60">
       <c r="A1" s="14" t="s">
         <v>38</v>
       </c>
@@ -1070,7 +1111,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1120,7 +1161,7 @@
         <v>1.1574074074074069E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
@@ -1170,7 +1211,7 @@
         <v>1.1574074074074069E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
@@ -1215,7 +1256,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
@@ -1260,7 +1301,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
@@ -1295,7 +1336,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="10"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="20" t="s">
         <v>5</v>
       </c>
@@ -1330,7 +1371,7 @@
       <c r="R7" s="13"/>
       <c r="S7" s="21"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8" s="9" t="s">
         <v>124</v>
       </c>
@@ -1380,7 +1421,7 @@
         <v>1.157407407407407E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="9" t="s">
         <v>125</v>
       </c>
@@ -1430,7 +1471,7 @@
         <v>1.157407407407407E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10" s="9" t="s">
         <v>6</v>
       </c>
@@ -1492,7 +1533,7 @@
         <v>1.4275079954526109</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
@@ -1539,7 +1580,7 @@
         <v>1.4275079954526109</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
@@ -1601,7 +1642,7 @@
         <v>1.4275079954526109</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13" s="9" t="s">
         <v>9</v>
       </c>
@@ -1648,7 +1689,7 @@
         <v>1.4275079954526109</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="9" t="s">
         <v>10</v>
       </c>
@@ -1695,7 +1736,7 @@
         <v>2.5027233520762868</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
@@ -1742,7 +1783,7 @@
         <v>2.5027233520762868</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" s="9" t="s">
         <v>12</v>
       </c>
@@ -1789,7 +1830,7 @@
         <v>2.5027233520762868</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="A17" s="9" t="s">
         <v>13</v>
       </c>
@@ -1836,7 +1877,7 @@
         <v>2.5027233520762868</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="A18" s="9" t="s">
         <v>14</v>
       </c>
@@ -1851,11 +1892,11 @@
       </c>
       <c r="E18" s="4">
         <f>E19/5</f>
-        <v>1.6399999999999999E-5</v>
+        <v>7.6467122800187402E-6</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" si="0"/>
-        <v>1.41696</v>
+        <v>0.66067594099361915</v>
       </c>
       <c r="G18" s="5">
         <v>0</v>
@@ -1881,11 +1922,11 @@
       </c>
       <c r="O18" s="5">
         <f t="shared" si="2"/>
-        <v>3.2799999999999999E-6</v>
+        <v>1.5293424560037481E-6</v>
       </c>
       <c r="P18" s="5">
         <f t="shared" si="3"/>
-        <v>8.1999999999999987E-5</v>
+        <v>3.8233561400093701E-5</v>
       </c>
       <c r="Q18" s="5" t="s">
         <v>67</v>
@@ -1897,7 +1938,7 @@
         <v>1.6399999999999997E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19">
       <c r="A19" s="9" t="s">
         <v>15</v>
       </c>
@@ -1911,11 +1952,11 @@
         <v>77</v>
       </c>
       <c r="E19" s="4">
-        <v>8.2000000000000001E-5</v>
+        <v>3.8233561400093701E-5</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" si="0"/>
-        <v>7.0848000000000004</v>
+        <v>3.3033797049680955</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -1931,11 +1972,11 @@
       </c>
       <c r="O19" s="5">
         <f t="shared" si="2"/>
-        <v>1.6399999999999999E-5</v>
+        <v>7.6467122800187402E-6</v>
       </c>
       <c r="P19" s="5">
         <f t="shared" si="3"/>
-        <v>4.0999999999999999E-4</v>
+        <v>1.9116780700046852E-4</v>
       </c>
       <c r="Q19" s="5" t="s">
         <v>67</v>
@@ -1947,7 +1988,7 @@
         <v>8.1999999999999998E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19">
       <c r="A20" s="9" t="s">
         <v>16</v>
       </c>
@@ -1962,11 +2003,11 @@
       </c>
       <c r="E20" s="4">
         <f>E21/5</f>
-        <v>1.2799999999999999E-5</v>
+        <v>5.3526985960131182E-5</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" si="0"/>
-        <v>1.1059199999999998</v>
+        <v>4.6247315869553347</v>
       </c>
       <c r="G20" s="5">
         <v>0</v>
@@ -1992,11 +2033,11 @@
       </c>
       <c r="O20" s="5">
         <f t="shared" si="2"/>
-        <v>2.5600000000000001E-6</v>
+        <v>1.0705397192026236E-5</v>
       </c>
       <c r="P20" s="5">
         <f t="shared" si="3"/>
-        <v>6.3999999999999997E-5</v>
+        <v>2.676349298006559E-4</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>67</v>
@@ -2008,7 +2049,7 @@
         <v>1.2799999999999999E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19">
       <c r="A21" s="9" t="s">
         <v>17</v>
       </c>
@@ -2022,11 +2063,12 @@
         <v>77</v>
       </c>
       <c r="E21" s="4">
-        <v>6.3999999999999997E-5</v>
+        <f>E19 * 7</f>
+        <v>2.676349298006559E-4</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="0"/>
-        <v>5.5296000000000003</v>
+        <v>23.12365793477667</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -2042,11 +2084,11 @@
       </c>
       <c r="O21" s="5">
         <f t="shared" si="2"/>
-        <v>1.2799999999999999E-5</v>
+        <v>5.3526985960131182E-5</v>
       </c>
       <c r="P21" s="5">
         <f t="shared" si="3"/>
-        <v>3.1999999999999997E-4</v>
+        <v>1.3381746490032794E-3</v>
       </c>
       <c r="Q21" s="5" t="s">
         <v>67</v>
@@ -2058,7 +2100,7 @@
         <v>6.3999999999999994E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="A22" s="9" t="s">
         <v>18</v>
       </c>
@@ -2072,11 +2114,12 @@
         <v>76</v>
       </c>
       <c r="E22" s="4">
-        <v>1.50462962962963E-5</v>
+        <f>0.0000962487421256466/2</f>
+        <v>4.8124371062823299E-5</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="0"/>
-        <v>1.3000000000000003</v>
+        <v>4.1579456598279325</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -2092,11 +2135,11 @@
       </c>
       <c r="O22" s="4">
         <f t="shared" ref="O22:O24" si="7">E22/10</f>
-        <v>1.5046296296296301E-6</v>
+        <v>4.8124371062823301E-6</v>
       </c>
       <c r="P22" s="4">
         <f t="shared" ref="P22:P24" si="8">E22*10</f>
-        <v>1.50462962962963E-4</v>
+        <v>4.8124371062823298E-4</v>
       </c>
       <c r="Q22" s="5" t="s">
         <v>67</v>
@@ -2108,7 +2151,7 @@
         <v>1.50462962962963E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="A23" s="9" t="s">
         <v>19</v>
       </c>
@@ -2122,11 +2165,12 @@
         <v>76</v>
       </c>
       <c r="E23" s="4">
-        <v>1.50462962962963E-5</v>
+        <f>E22</f>
+        <v>4.8124371062823299E-5</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" si="0"/>
-        <v>1.3000000000000003</v>
+        <v>4.1579456598279325</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -2142,11 +2186,11 @@
       </c>
       <c r="O23" s="4">
         <f t="shared" si="7"/>
-        <v>1.5046296296296301E-6</v>
+        <v>4.8124371062823301E-6</v>
       </c>
       <c r="P23" s="4">
         <f t="shared" si="8"/>
-        <v>1.50462962962963E-4</v>
+        <v>4.8124371062823298E-4</v>
       </c>
       <c r="Q23" s="5" t="s">
         <v>67</v>
@@ -2158,7 +2202,7 @@
         <v>1.50462962962963E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="A24" s="9" t="s">
         <v>20</v>
       </c>
@@ -2172,11 +2216,12 @@
         <v>76</v>
       </c>
       <c r="E24" s="4">
-        <v>6.7708333333333344E-5</v>
+        <f>E23*4.5</f>
+        <v>2.1655966978270484E-4</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" si="0"/>
-        <v>5.8500000000000014</v>
+        <v>18.710755469225699</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -2192,11 +2237,11 @@
       </c>
       <c r="O24" s="4">
         <f t="shared" si="7"/>
-        <v>6.7708333333333347E-6</v>
+        <v>2.1655966978270485E-5</v>
       </c>
       <c r="P24" s="4">
         <f t="shared" si="8"/>
-        <v>6.7708333333333346E-4</v>
+        <v>2.1655966978270484E-3</v>
       </c>
       <c r="Q24" s="5" t="s">
         <v>67</v>
@@ -2208,7 +2253,7 @@
         <v>6.7708333333333346E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19">
       <c r="A25" s="9" t="s">
         <v>21</v>
       </c>
@@ -2246,7 +2291,7 @@
       <c r="R25" s="5"/>
       <c r="S25" s="10"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19">
       <c r="A26" s="9" t="s">
         <v>128</v>
       </c>
@@ -2293,7 +2338,7 @@
       <c r="R26" s="5"/>
       <c r="S26" s="10"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19">
       <c r="A27" s="9" t="s">
         <v>22</v>
       </c>
@@ -2353,7 +2398,7 @@
         <v>6.4814814814814812E-6</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19">
       <c r="A28" s="9" t="s">
         <v>23</v>
       </c>
@@ -2413,7 +2458,7 @@
         <v>4.050925925925926E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19">
       <c r="A29" s="9" t="s">
         <v>92</v>
       </c>
@@ -2473,7 +2518,7 @@
         <v>7.6967592592592601E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19">
       <c r="A30" s="9" t="s">
         <v>24</v>
       </c>
@@ -2535,7 +2580,7 @@
         <v>2.5027233520762868</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19">
       <c r="A31" s="9" t="s">
         <v>25</v>
       </c>
@@ -2603,7 +2648,7 @@
         <v>1.1574074074074074E-6</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19">
       <c r="A32" s="22" t="s">
         <v>104</v>
       </c>
@@ -2651,7 +2696,7 @@
       <c r="R32" s="5"/>
       <c r="S32" s="10"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19">
       <c r="A33" s="22" t="s">
         <v>106</v>
       </c>
@@ -2699,7 +2744,7 @@
       <c r="R33" s="5"/>
       <c r="S33" s="10"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19">
       <c r="A34" s="22" t="s">
         <v>105</v>
       </c>
@@ -2734,7 +2779,7 @@
       <c r="R34" s="5"/>
       <c r="S34" s="10"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19">
       <c r="A35" s="22" t="s">
         <v>107</v>
       </c>
@@ -2784,7 +2829,7 @@
       <c r="R35" s="5"/>
       <c r="S35" s="10"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19">
       <c r="A36" s="9" t="s">
         <v>26</v>
       </c>
@@ -2849,7 +2894,7 @@
         <v>1.4275079954526109</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19">
       <c r="A37" s="9" t="s">
         <v>27</v>
       </c>
@@ -2914,7 +2959,7 @@
         <v>1.4275079954526109</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19">
       <c r="A38" s="9" t="s">
         <v>28</v>
       </c>
@@ -2976,7 +3021,7 @@
         <v>6.4814814814814797E-16</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19">
       <c r="A39" s="9" t="s">
         <v>29</v>
       </c>
@@ -3038,7 +3083,7 @@
         <v>4.0509259259259247E-16</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19">
       <c r="A40" s="9" t="s">
         <v>30</v>
       </c>
@@ -3103,7 +3148,7 @@
         <v>1.1574074074074074E-6</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19">
       <c r="A41" s="9" t="s">
         <v>31</v>
       </c>
@@ -3168,7 +3213,7 @@
         <v>1.1574074074074074E-6</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19">
       <c r="A42" s="9" t="s">
         <v>32</v>
       </c>
@@ -3230,7 +3275,7 @@
         <v>1.1574074074074101E-6</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19">
       <c r="A43" s="9" t="s">
         <v>33</v>
       </c>
@@ -3292,7 +3337,7 @@
         <v>1.1574074074074101E-6</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19">
       <c r="A44" s="9" t="s">
         <v>34</v>
       </c>
@@ -3330,7 +3375,7 @@
       <c r="R44" s="5"/>
       <c r="S44" s="10"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19">
       <c r="A45" s="9" t="s">
         <v>35</v>
       </c>
@@ -3368,7 +3413,7 @@
       <c r="R45" s="5"/>
       <c r="S45" s="10"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19">
       <c r="A46" s="9" t="s">
         <v>36</v>
       </c>
@@ -3403,7 +3448,7 @@
       <c r="R46" s="5"/>
       <c r="S46" s="10"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19">
       <c r="A47" s="9" t="s">
         <v>37</v>
       </c>
@@ -3438,7 +3483,7 @@
       <c r="R47" s="5"/>
       <c r="S47" s="10"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19">
       <c r="A48" s="22" t="s">
         <v>95</v>
       </c>
@@ -3473,7 +3518,7 @@
       <c r="R48" s="5"/>
       <c r="S48" s="10"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19">
       <c r="A49" s="22" t="s">
         <v>96</v>
       </c>
@@ -3508,7 +3553,7 @@
       <c r="R49" s="5"/>
       <c r="S49" s="10"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19">
       <c r="A50" s="22" t="s">
         <v>97</v>
       </c>
@@ -3543,7 +3588,7 @@
       <c r="R50" s="5"/>
       <c r="S50" s="10"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19">
       <c r="A51" s="22" t="s">
         <v>98</v>
       </c>
@@ -3578,7 +3623,7 @@
       <c r="R51" s="5"/>
       <c r="S51" s="10"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19">
       <c r="A52" s="22" t="s">
         <v>103</v>
       </c>
@@ -3616,7 +3661,7 @@
       <c r="R52" s="5"/>
       <c r="S52" s="10"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19">
       <c r="A53" s="22" t="s">
         <v>114</v>
       </c>
@@ -3654,7 +3699,7 @@
       <c r="R53" s="5"/>
       <c r="S53" s="10"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19">
       <c r="A54" s="22" t="s">
         <v>108</v>
       </c>
@@ -3702,7 +3747,7 @@
       <c r="R54" s="5"/>
       <c r="S54" s="10"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19">
       <c r="A55" s="23" t="s">
         <v>109</v>
       </c>
@@ -3750,7 +3795,7 @@
       <c r="R55" s="27"/>
       <c r="S55" s="28"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19">
       <c r="A56" s="29" t="s">
         <v>119</v>
       </c>
@@ -3785,7 +3830,7 @@
       <c r="R56" s="5"/>
       <c r="S56" s="5"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19">
       <c r="A57" s="29" t="s">
         <v>120</v>
       </c>
@@ -3820,7 +3865,7 @@
       <c r="R57" s="5"/>
       <c r="S57" s="5"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19">
       <c r="A58" s="29" t="s">
         <v>126</v>
       </c>
@@ -3855,7 +3900,7 @@
       <c r="R58" s="5"/>
       <c r="S58" s="5"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19">
       <c r="A59" s="29" t="s">
         <v>127</v>
       </c>
@@ -3889,6 +3934,159 @@
       <c r="Q59" s="5"/>
       <c r="R59" s="5"/>
       <c r="S59" s="5"/>
+    </row>
+    <row r="60" spans="1:19">
+      <c r="A60" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E60" s="32">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="N60" s="33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19">
+      <c r="A61" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E61" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F61" s="10"/>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61" t="s">
+        <v>67</v>
+      </c>
+      <c r="N61" t="s">
+        <v>66</v>
+      </c>
+      <c r="O61" s="34">
+        <f t="shared" ref="O61:O62" si="19">E61/10</f>
+        <v>1E-3</v>
+      </c>
+      <c r="P61" s="34">
+        <f t="shared" ref="P61:P62" si="20">E61*10</f>
+        <v>0.1</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>67</v>
+      </c>
+      <c r="R61">
+        <v>1E-3</v>
+      </c>
+      <c r="S61">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19">
+      <c r="A62" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E62" s="5">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F62" s="10"/>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62" t="s">
+        <v>66</v>
+      </c>
+      <c r="N62" t="s">
+        <v>67</v>
+      </c>
+      <c r="O62" s="34">
+        <f t="shared" si="19"/>
+        <v>1.0000000000000002E-6</v>
+      </c>
+      <c r="P62" s="34">
+        <f t="shared" si="20"/>
+        <v>1E-4</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>67</v>
+      </c>
+      <c r="R62">
+        <v>1.0000000000000002E-6</v>
+      </c>
+      <c r="S62">
+        <v>1E-4</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:S55" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
@@ -3906,17 +4104,17 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:6">
       <c r="D19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:6">
       <c r="D20">
         <v>0.7</v>
       </c>
@@ -3924,7 +4122,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:6">
       <c r="D21">
         <f>D20/ 100</f>
         <v>6.9999999999999993E-3</v>
@@ -3936,7 +4134,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:6">
       <c r="D22">
         <f>D21/3600</f>
         <v>1.9444444444444444E-6</v>
@@ -3949,7 +4147,7 @@
         <v>5.75E-6</v>
       </c>
     </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:6">
       <c r="D23">
         <f>0.3/D22</f>
         <v>154285.71428571429</v>

</xml_diff>